<commit_message>
minor changes to excel file
</commit_message>
<xml_diff>
--- a/PractiseBdd/TestData/TestData.xlsx
+++ b/PractiseBdd/TestData/TestData.xlsx
@@ -1,16 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NEELA\OneDrive\Desktop\Tasks\MakeMyTripWithBDDApproach\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E2AEEA-F2E5-405E-8835-834149943F24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{6F4C887D-6661-457B-BA4A-5716A4CEC213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="20760" windowHeight="14625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Navbardata" sheetId="1" r:id="rId1"/>
@@ -22,6 +17,7 @@
     <sheet name="moreOptions" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:V39"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -447,7 +443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -709,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6945D62D-E99C-45BF-B68B-73E6F9D21AB8}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>